<commit_message>
Final burndown chart for Sprint 2
</commit_message>
<xml_diff>
--- a/sprints/sprint 2/Burndown Chart Sprint 2.xlsx
+++ b/sprints/sprint 2/Burndown Chart Sprint 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azeldaniel/Documents/UWI/Year 3/Semester 1/COMP 3613/project/swe2-project/sprints/sprint 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D640F15A-5DDA-DB4C-96DE-F8867E91F507}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDC541B-C67F-7741-8FB2-98CC95BBC488}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" xr2:uid="{583FEC89-0C8D-4923-A5A2-4ADAB6A20CAF}"/>
   </bookViews>
@@ -269,9 +269,6 @@
                 <c:pt idx="14">
                   <c:v>43430</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>43431</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -322,6 +319,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -410,9 +410,6 @@
                 <c:pt idx="14">
                   <c:v>43430</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>43431</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -426,49 +423,46 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67.2</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.400000000000006</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.600000000000009</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.800000000000011</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.000000000000014</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.200000000000017</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.40000000000002</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.600000000000023</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>28.800000000000022</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24.000000000000021</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.200000000000021</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14.40000000000002</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.6000000000000192</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.8000000000000194</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.9539925233402755E-14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,7 +1572,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1631,8 +1625,8 @@
         <v>72</v>
       </c>
       <c r="C3" s="3">
-        <f>C2-4.8</f>
-        <v>67.2</v>
+        <f>C2-5</f>
+        <v>67</v>
       </c>
       <c r="U3" t="s">
         <v>1</v>
@@ -1653,8 +1647,8 @@
         <v>60</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" ref="C4:C17" si="1">C3-4.8</f>
-        <v>62.400000000000006</v>
+        <f t="shared" ref="C4:C16" si="1">C3-5</f>
+        <v>62</v>
       </c>
       <c r="U4" t="s">
         <v>2</v>
@@ -1676,7 +1670,7 @@
       </c>
       <c r="C5" s="3">
         <f t="shared" si="1"/>
-        <v>57.600000000000009</v>
+        <v>57</v>
       </c>
       <c r="U5" t="s">
         <v>3</v>
@@ -1698,7 +1692,7 @@
       </c>
       <c r="C6" s="3">
         <f t="shared" si="1"/>
-        <v>52.800000000000011</v>
+        <v>52</v>
       </c>
       <c r="U6" t="s">
         <v>4</v>
@@ -1720,7 +1714,7 @@
       </c>
       <c r="C7" s="3">
         <f t="shared" si="1"/>
-        <v>48.000000000000014</v>
+        <v>47</v>
       </c>
       <c r="V7">
         <f>SUM(V2:V6)</f>
@@ -1740,7 +1734,7 @@
       </c>
       <c r="C8" s="3">
         <f t="shared" si="1"/>
-        <v>43.200000000000017</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
@@ -1752,7 +1746,7 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" si="1"/>
-        <v>38.40000000000002</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
@@ -1764,7 +1758,7 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" si="1"/>
-        <v>33.600000000000023</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
@@ -1776,7 +1770,7 @@
       </c>
       <c r="C11" s="3">
         <f t="shared" si="1"/>
-        <v>28.800000000000022</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
@@ -1788,7 +1782,7 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" si="1"/>
-        <v>24.000000000000021</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
@@ -1800,7 +1794,7 @@
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>19.200000000000021</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -1812,7 +1806,7 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" si="1"/>
-        <v>14.40000000000002</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -1824,26 +1818,23 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" si="1"/>
-        <v>9.6000000000000192</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43430</v>
       </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
       <c r="C16" s="3">
-        <f t="shared" si="1"/>
-        <v>4.8000000000000194</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>43431</v>
-      </c>
-      <c r="C17" s="3">
-        <f t="shared" si="1"/>
-        <v>1.9539925233402755E-14</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>

</xml_diff>